<commit_message>
steps used in excel sheet
</commit_message>
<xml_diff>
--- a/assignment -10mar2025.xlsx
+++ b/assignment -10mar2025.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28627"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="282" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33AA4DEB-6A14-4467-8A40-6FC68B7AC1EE}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRAVEEN\Documents\Data analyst\Excel\Excel-project-01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C7608B-580E-4C61-8FE7-EC279AB8A853}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,12 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,14 +31,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
   <si>
     <t>Abi</t>
   </si>
@@ -232,13 +231,43 @@
   </si>
   <si>
     <t>kind</t>
+  </si>
+  <si>
+    <t>JANUARY</t>
+  </si>
+  <si>
+    <t>MARCH</t>
+  </si>
+  <si>
+    <t>AUGUST</t>
+  </si>
+  <si>
+    <t>DECEMBER</t>
+  </si>
+  <si>
+    <t>email add</t>
+  </si>
+  <si>
+    <t>total add</t>
+  </si>
+  <si>
+    <t>sathis123@gmail.com</t>
+  </si>
+  <si>
+    <t>sathis234@gmail.com</t>
+  </si>
+  <si>
+    <t>sathis345@gmail.com</t>
+  </si>
+  <si>
+    <t>sathis456@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +287,12 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -287,7 +322,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -336,11 +371,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -380,6 +430,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,12 +778,12 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" ht="14.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,7 +802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" ht="14.4">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -756,7 +814,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" ht="14.4">
       <c r="B5" s="1">
         <v>4800</v>
       </c>
@@ -767,7 +825,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" ht="14.4">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -778,7 +836,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" ht="14.4">
       <c r="B7" s="1">
         <v>2480</v>
       </c>
@@ -789,7 +847,7 @@
         <v>3510</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" ht="14.4">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -800,7 +858,7 @@
         <v>4580</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" ht="14.4">
       <c r="B9" s="1">
         <v>3510</v>
       </c>
@@ -811,7 +869,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" ht="14.4">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
@@ -822,7 +880,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" ht="14.4">
       <c r="B11" s="1">
         <v>4580</v>
       </c>
@@ -833,7 +891,7 @@
         <v>4530</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" ht="14.4">
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -844,41 +902,41 @@
         <v>3240</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" ht="14.4">
       <c r="B13" s="1">
         <v>3300</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:5" ht="14.4">
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:5" ht="14.4">
       <c r="B15" s="1">
         <v>1950</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:5" ht="14.4">
       <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" ht="14.4">
       <c r="B17" s="1">
         <v>4530</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" ht="14.4">
       <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" ht="14.4">
       <c r="B19" s="1">
         <v>3240</v>
       </c>
@@ -890,18 +948,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073A81D1-2F7B-4CDB-AAB8-5B8B9DA35D61}">
-  <dimension ref="A3:G48"/>
+  <dimension ref="A3:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:G48"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="3" max="3" width="13.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.59765625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3984375" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="77" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:7">
@@ -1043,8 +1101,8 @@
         <v>25</v>
       </c>
       <c r="G17" s="11" t="str">
-        <f>_xlfn.CONCAT(C17," ",D17," - ",E17)</f>
-        <v>Praveen Kumar - 25</v>
+        <f>CONCATENATE(C17," ",D17," , ",E17)</f>
+        <v>Praveen Kumar , 25</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1058,8 +1116,8 @@
         <v>18</v>
       </c>
       <c r="G18" s="11" t="str">
-        <f t="shared" ref="G18:G19" si="1">_xlfn.CONCAT(C18," ",D18," - ",E18)</f>
-        <v>Sam Asron - 18</v>
+        <f t="shared" ref="G18:G19" si="1">CONCATENATE(C18," ",D18," , ",E18)</f>
+        <v>Sam Asron , 18</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1074,7 +1132,7 @@
       </c>
       <c r="G19" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>Sanjay Diwahar - 20</v>
+        <v>Sanjay Diwahar , 20</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1132,10 +1190,10 @@
         <v>5</v>
       </c>
       <c r="C30" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="13" t="s">
         <v>36</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>38</v>
@@ -1146,62 +1204,62 @@
     </row>
     <row r="31" spans="1:7">
       <c r="C31" s="11">
-        <v>1</v>
-      </c>
-      <c r="D31" s="11">
         <v>8</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="E31" s="11">
         <v>2004</v>
       </c>
-      <c r="G31" s="15">
-        <f>DATE(E31,C31,D31)</f>
-        <v>37994</v>
+      <c r="G31" s="15" t="str">
+        <f>CONCATENATE(C31," - ",D31," - ",E31)</f>
+        <v>8 - JANUARY - 2004</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="C32" s="11">
-        <v>3</v>
-      </c>
-      <c r="D32" s="11">
         <v>15</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="E32" s="11">
         <v>2008</v>
       </c>
-      <c r="G32" s="15">
-        <f t="shared" ref="G32:G34" si="3">DATE(E32,C32,D32)</f>
-        <v>39522</v>
+      <c r="G32" s="15" t="str">
+        <f t="shared" ref="G32:G34" si="3">CONCATENATE(C32," - ",D32," - ",E32)</f>
+        <v>15 - MARCH - 2008</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="C33" s="11">
-        <v>8</v>
-      </c>
-      <c r="D33" s="11">
         <v>6</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="E33" s="11">
         <v>2010</v>
       </c>
-      <c r="G33" s="15">
+      <c r="G33" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>40396</v>
+        <v>6 - AUGUST - 2010</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="C34" s="11">
-        <v>12</v>
-      </c>
-      <c r="D34" s="11">
         <v>24</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="E34" s="11">
         <v>2015</v>
       </c>
-      <c r="G34" s="15">
+      <c r="G34" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>42362</v>
+        <v>24 - DECEMBER - 2015</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1316,7 +1374,43 @@
         <v>You are kind</v>
       </c>
     </row>
+    <row r="52" spans="1:7">
+      <c r="A52">
+        <v>8</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G52" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="C53" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" s="20" t="str">
+        <f>CONCATENATE(C53," , ",C54," , ",C55," , ",C56)</f>
+        <v>sathis123@gmail.com , sathis234@gmail.com , sathis345@gmail.com , sathis456@gmail.com</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="C54" s="22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="C55" s="22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="C56" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>